<commit_message>
Final updates for the final turn in with statistics
</commit_message>
<xml_diff>
--- a/doc/StitchingTime.xlsx
+++ b/doc/StitchingTime.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IMG" sheetId="1" r:id="rId1"/>
+    <sheet name="OCR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Image stitching time</t>
   </si>
@@ -43,12 +44,36 @@
   <si>
     <t>Final image size (MB)</t>
   </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Partial Success</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>% success</t>
+  </si>
+  <si>
+    <t>% some success</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +86,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,10 +127,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -106,9 +139,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,7 +180,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -157,14 +193,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
               <a:t>Image</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
               <a:t> Stitching size verse time</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -182,7 +218,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -209,7 +245,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>IMG!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -232,7 +268,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>IMG!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -294,7 +330,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>IMG!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -367,7 +403,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>IMG!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -403,7 +439,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$11</c:f>
+              <c:f>IMG!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -617,6 +653,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="338511216"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1260,15 +1297,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1555,7 +1592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" activeCellId="1" sqref="A1 P11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1749,4 +1788,95 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f>19-C2</f>
+        <v>14</v>
+      </c>
+      <c r="E2" s="4">
+        <f>B2/SUM(B2:D2)</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F2" s="4">
+        <f>(B2+C2)/SUM(B2:D2)</f>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <f>B3/SUM(B3:D3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <f>(B3+C3)/SUM(B3:D3)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f>(B2+B3)/SUM(B2:D3)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <f>SUM(B2:C3)/SUM(B2:D3)</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>